<commit_message>
Mise à jour du projet
</commit_message>
<xml_diff>
--- a/RESULTAT_2024.xlsx
+++ b/RESULTAT_2024.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>STATIONS</t>
   </si>
@@ -186,36 +186,6 @@
   </si>
   <si>
     <t>Tienko</t>
-  </si>
-  <si>
-    <t>Bediala</t>
-  </si>
-  <si>
-    <t>Dianra</t>
-  </si>
-  <si>
-    <t>Kani</t>
-  </si>
-  <si>
-    <t>Mankono</t>
-  </si>
-  <si>
-    <t>Sarhala</t>
-  </si>
-  <si>
-    <t>Séguéla_CIDT</t>
-  </si>
-  <si>
-    <t>Tengrela</t>
-  </si>
-  <si>
-    <t>Vavoua</t>
-  </si>
-  <si>
-    <t>Worofla</t>
-  </si>
-  <si>
-    <t>Zuenoula</t>
   </si>
   <si>
     <t>Touba</t>
@@ -451,7 +421,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="37">
     <font>
       <sz val="11.000000"/>
       <color theme="1" tint="0"/>
@@ -515,11 +485,6 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -593,7 +558,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -618,7 +582,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -661,12 +624,10 @@
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Arial Narrow"/>
     </font>
     <font>
       <sz val="8.000000"/>
-      <color indexed="64"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -1158,19 +1119,19 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="167" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="9" fillId="29" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="10" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="30" borderId="3" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="12" fillId="31" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="13" fillId="26" borderId="4" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="11" fillId="31" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="12" fillId="26" borderId="4" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="13" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="14" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="15" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="16" fillId="0" borderId="5" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="17" fillId="0" borderId="6" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="18" fillId="0" borderId="7" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="19" fillId="0" borderId="8" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="20" fillId="32" borderId="9" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="15" fillId="0" borderId="5" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="16" fillId="0" borderId="6" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="17" fillId="0" borderId="7" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="18" fillId="0" borderId="8" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="19" fillId="32" borderId="9" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="69">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -1178,52 +1139,52 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="19" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="18" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="33" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="34" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="35" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="36" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="23" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="22" fillId="0" borderId="3" numFmtId="0" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="21" fillId="0" borderId="3" numFmtId="0" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf fontId="23" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1"/>
     <xf fontId="24" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="25" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="26" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="25" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="27" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="28" fillId="0" borderId="0" numFmtId="0" xfId="38" applyFont="1"/>
-    <xf fontId="29" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="11" fillId="0" borderId="3" numFmtId="0" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="26" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="27" fillId="0" borderId="0" numFmtId="0" xfId="38" applyFont="1"/>
+    <xf fontId="28" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="10" fillId="0" borderId="3" numFmtId="0" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="30" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="29" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="31" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="22" fillId="0" borderId="3" numFmtId="0" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="30" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="21" fillId="0" borderId="3" numFmtId="0" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="32" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="31" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="37" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf fontId="0" fillId="38" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf fontId="0" fillId="39" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
@@ -1233,37 +1194,37 @@
     <xf fontId="10" fillId="0" borderId="11" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="33" fillId="0" borderId="12" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="32" fillId="0" borderId="12" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="33" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="32" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="34" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="33" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="34" fillId="0" borderId="11" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="33" fillId="0" borderId="11" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="35" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="34" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="11" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="37" borderId="11" numFmtId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="35" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="34" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="10" fillId="0" borderId="14" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="33" fillId="0" borderId="13" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="32" fillId="0" borderId="13" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="33" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="32" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="34" fillId="0" borderId="14" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="33" fillId="0" borderId="14" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="14" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1282,7 +1243,7 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="16" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="34" fillId="0" borderId="15" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="33" fillId="0" borderId="15" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="37" borderId="15" numFmtId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1295,11 +1256,11 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="36" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="35" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="38" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="38" applyFont="1"/>
     <xf fontId="0" fillId="35" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="37" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="36" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
@@ -1863,7 +1824,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="100" workbookViewId="0">
       <selection activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -2395,11 +2356,6 @@
       <c r="H17" s="12">
         <v>58.100000000000009</v>
       </c>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
     </row>
     <row r="18" ht="14.4" customHeight="1">
       <c r="A18" s="18" t="s">
@@ -3332,371 +3288,128 @@
       <c r="M47" s="13"/>
     </row>
     <row r="48" ht="14.4" customHeight="1">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="28" t="s">
         <v>54</v>
       </c>
       <c r="B48" s="9">
-        <v>-6.3035300000000003</v>
+        <v>-7.6833330000000002</v>
       </c>
       <c r="C48" s="9">
-        <v>7.1739600000000001</v>
-      </c>
-      <c r="D48" s="10">
-        <v>29.066451612903236</v>
+        <v>8.2833330000000007</v>
+      </c>
+      <c r="D48" s="11">
+        <v>28.5</v>
       </c>
       <c r="E48" s="11">
-        <v>22.100000000000001</v>
+        <v>22.300000000000001</v>
       </c>
       <c r="F48" s="10">
-        <v>149.52000000000001</v>
-      </c>
-      <c r="G48" s="11">
-        <v>84.93793103448273</v>
+        <v>101.01000000000001</v>
+      </c>
+      <c r="G48" s="17">
+        <v>90.70714285714287</v>
       </c>
       <c r="H48" s="12">
-        <v>61.899999999999991</v>
-      </c>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
+        <v>90.199999999999989</v>
+      </c>
     </row>
     <row r="49" ht="14.4" customHeight="1">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B49" s="9">
-        <v>-6.25</v>
+        <v>-7.516667</v>
       </c>
       <c r="C49" s="9">
-        <v>8.75</v>
-      </c>
-      <c r="D49" s="10">
-        <v>29.199999999999999</v>
+        <v>7.3833330000000004</v>
+      </c>
+      <c r="D49" s="11">
+        <v>28.5</v>
       </c>
       <c r="E49" s="11">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="F49" s="10">
-        <v>144.04999999999998</v>
-      </c>
-      <c r="G49" s="10">
-        <v>88.680000000000021</v>
+        <v>22.300000000000001</v>
+      </c>
+      <c r="F49" s="15">
+        <v>369.5</v>
+      </c>
+      <c r="G49" s="17">
+        <v>90.70714285714287</v>
       </c>
       <c r="H49" s="12">
-        <v>128.40000000000003</v>
-      </c>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
+        <v>90.199999999999989</v>
+      </c>
     </row>
     <row r="50" ht="14.4" customHeight="1">
-      <c r="A50" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="9">
-        <v>-6.5999999999999996</v>
-      </c>
-      <c r="C50" s="9">
-        <v>8.4666669999999993</v>
-      </c>
-      <c r="D50" s="10">
-        <v>29.199999999999999</v>
-      </c>
-      <c r="E50" s="11">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="F50" s="10">
-        <v>142.14999999999998</v>
-      </c>
-      <c r="G50" s="10">
-        <v>88.680000000000021</v>
-      </c>
-      <c r="H50" s="12">
-        <v>128.40000000000003</v>
-      </c>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
     </row>
     <row r="51" ht="14.4" customHeight="1">
-      <c r="A51" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="9">
-        <v>-6.1833330000000002</v>
-      </c>
-      <c r="C51" s="9">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="D51" s="10">
-        <v>29.199999999999999</v>
-      </c>
-      <c r="E51" s="11">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="F51" s="10">
-        <v>124.28999999999999</v>
-      </c>
-      <c r="G51" s="10">
-        <v>88.680000000000021</v>
-      </c>
-      <c r="H51" s="12">
-        <v>128.40000000000003</v>
-      </c>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" ht="14.4" customHeight="1">
-      <c r="A52" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="9">
-        <v>-6.1666670000000003</v>
-      </c>
-      <c r="C52" s="9">
-        <v>8.4166670000000003</v>
-      </c>
-      <c r="D52" s="10">
-        <v>29.199999999999999</v>
-      </c>
-      <c r="E52" s="11">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="F52" s="10">
-        <v>129.69999999999999</v>
-      </c>
-      <c r="G52" s="10">
-        <v>88.680000000000021</v>
-      </c>
-      <c r="H52" s="12">
-        <v>128.40000000000003</v>
-      </c>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
     </row>
     <row r="53" ht="14.4" customHeight="1">
-      <c r="A53" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="9">
-        <v>-6.6666670000000003</v>
-      </c>
-      <c r="C53" s="9">
-        <v>7.9500000000000002</v>
-      </c>
-      <c r="D53" s="10">
-        <v>28.5</v>
-      </c>
-      <c r="E53" s="11">
-        <v>22.300000000000001</v>
-      </c>
-      <c r="F53" s="10">
-        <v>125.88</v>
-      </c>
-      <c r="G53" s="17">
-        <v>90.70714285714287</v>
-      </c>
-      <c r="H53" s="12">
-        <v>90.199999999999989</v>
-      </c>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
     </row>
     <row r="54" ht="14.4" customHeight="1">
-      <c r="A54" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="9">
-        <v>-6.4000000000000004</v>
-      </c>
-      <c r="C54" s="9">
-        <v>10.483333</v>
-      </c>
-      <c r="D54" s="10">
-        <v>29.199999999999999</v>
-      </c>
-      <c r="E54" s="11">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="F54" s="10">
-        <v>225.22999999999999</v>
-      </c>
-      <c r="G54" s="10">
-        <v>88.680000000000021</v>
-      </c>
-      <c r="H54" s="12">
-        <v>128.40000000000003</v>
-      </c>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
     </row>
     <row r="55" ht="14.4" customHeight="1">
-      <c r="A55" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="9">
-        <v>-6.4666670000000002</v>
-      </c>
-      <c r="C55" s="9">
-        <v>7.3666669999999996</v>
-      </c>
-      <c r="D55" s="11">
-        <v>28.5</v>
-      </c>
-      <c r="E55" s="11">
-        <v>22.300000000000001</v>
-      </c>
-      <c r="F55" s="10">
-        <v>100.74000000000001</v>
-      </c>
-      <c r="G55" s="17">
-        <v>90.70714285714287</v>
-      </c>
-      <c r="H55" s="12">
-        <v>90.199999999999989</v>
-      </c>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
     </row>
     <row r="56" ht="14.4" customHeight="1">
-      <c r="A56" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B56" s="9">
-        <v>-6.9000000000000004</v>
-      </c>
-      <c r="C56" s="9">
-        <v>8.266667</v>
-      </c>
-      <c r="D56" s="11">
-        <v>28.5</v>
-      </c>
-      <c r="E56" s="11">
-        <v>22.300000000000001</v>
-      </c>
-      <c r="F56" s="10">
-        <v>132.60000000000002</v>
-      </c>
-      <c r="G56" s="17">
-        <v>90.70714285714287</v>
-      </c>
-      <c r="H56" s="12">
-        <v>90.199999999999989</v>
-      </c>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
     </row>
     <row r="57" ht="14.4" customHeight="1">
-      <c r="A57" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="9">
-        <v>-6.0499999999999998</v>
-      </c>
-      <c r="C57" s="9">
-        <v>7.4166670000000003</v>
-      </c>
-      <c r="D57" s="17">
-        <v>29.066451612903236</v>
-      </c>
-      <c r="E57" s="11">
-        <v>22.100000000000001</v>
-      </c>
-      <c r="F57" s="10">
-        <v>178.71999999999997</v>
-      </c>
-      <c r="G57" s="11">
-        <v>84.93793103448273</v>
-      </c>
-      <c r="H57" s="12">
-        <v>61.899999999999991</v>
-      </c>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
-      <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
     </row>
     <row r="58" ht="14.4" customHeight="1">
-      <c r="A58" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="9">
-        <v>-7.6833330000000002</v>
-      </c>
-      <c r="C58" s="9">
-        <v>8.2833330000000007</v>
-      </c>
-      <c r="D58" s="11">
-        <v>28.5</v>
-      </c>
-      <c r="E58" s="11">
-        <v>22.300000000000001</v>
-      </c>
-      <c r="F58" s="10">
-        <v>101.01000000000001</v>
-      </c>
-      <c r="G58" s="17">
-        <v>90.70714285714287</v>
-      </c>
-      <c r="H58" s="12">
-        <v>90.199999999999989</v>
-      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
     </row>
     <row r="59" ht="14.4" customHeight="1">
-      <c r="A59" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B59" s="9">
-        <v>-7.516667</v>
-      </c>
-      <c r="C59" s="9">
-        <v>7.3833330000000004</v>
-      </c>
-      <c r="D59" s="11">
-        <v>28.5</v>
-      </c>
-      <c r="E59" s="11">
-        <v>22.300000000000001</v>
-      </c>
-      <c r="F59" s="15">
-        <v>369.5</v>
-      </c>
-      <c r="G59" s="17">
-        <v>90.70714285714287</v>
-      </c>
-      <c r="H59" s="12">
-        <v>90.199999999999989</v>
-      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="60" ht="14.4" customHeight="1">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="13"/>
@@ -3704,9 +3417,6 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" ht="14.4" customHeight="1">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="13"/>
@@ -3714,9 +3424,6 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" ht="14.4" customHeight="1">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="13"/>
@@ -3724,9 +3431,6 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" ht="14.4" customHeight="1">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="13"/>
@@ -3734,9 +3438,6 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" ht="14.4" customHeight="1">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="13"/>
@@ -3744,9 +3445,6 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" ht="14.4" customHeight="1">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="13"/>
@@ -3754,9 +3452,6 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" ht="14.4" customHeight="1">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="13"/>
@@ -3764,9 +3459,6 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" ht="14.4" customHeight="1">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="13"/>
@@ -3774,9 +3466,6 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" ht="14.4" customHeight="1">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="13"/>
@@ -3784,9 +3473,6 @@
       <c r="H68" s="13"/>
     </row>
     <row r="69" ht="14.4" customHeight="1">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="13"/>
@@ -3794,9 +3480,6 @@
       <c r="H69" s="13"/>
     </row>
     <row r="70" ht="14.4" customHeight="1">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="13"/>
@@ -3804,9 +3487,6 @@
       <c r="H70" s="13"/>
     </row>
     <row r="71" ht="14.4" customHeight="1">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="13"/>
@@ -3814,9 +3494,6 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" ht="14.4" customHeight="1">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="13"/>
@@ -3824,9 +3501,6 @@
       <c r="H72" s="13"/>
     </row>
     <row r="73" ht="14.4" customHeight="1">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="13"/>
@@ -3834,9 +3508,6 @@
       <c r="H73" s="13"/>
     </row>
     <row r="74" ht="14.4" customHeight="1">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="13"/>
@@ -3844,9 +3515,6 @@
       <c r="H74" s="13"/>
     </row>
     <row r="75" ht="14.4" customHeight="1">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="13"/>
@@ -3854,9 +3522,6 @@
       <c r="H75" s="13"/>
     </row>
     <row r="76" ht="14.4" customHeight="1">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="13"/>
@@ -3864,9 +3529,6 @@
       <c r="H76" s="13"/>
     </row>
     <row r="77" ht="14.4" customHeight="1">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="13"/>
@@ -3874,9 +3536,6 @@
       <c r="H77" s="13"/>
     </row>
     <row r="78" ht="14.4" customHeight="1">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="13"/>
@@ -3884,9 +3543,6 @@
       <c r="H78" s="13"/>
     </row>
     <row r="79" ht="14.4" customHeight="1">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="13"/>
@@ -3894,9 +3550,6 @@
       <c r="H79" s="13"/>
     </row>
     <row r="80" ht="14.4" customHeight="1">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="13"/>
@@ -3904,9 +3557,6 @@
       <c r="H80" s="13"/>
     </row>
     <row r="81" ht="14.4" customHeight="1">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="13"/>
@@ -3914,9 +3564,6 @@
       <c r="H81" s="13"/>
     </row>
     <row r="82" ht="14.4" customHeight="1">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="13"/>
@@ -3924,9 +3571,6 @@
       <c r="H82" s="13"/>
     </row>
     <row r="83" ht="14.4" customHeight="1">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="13"/>
@@ -3934,9 +3578,6 @@
       <c r="H83" s="13"/>
     </row>
     <row r="84" ht="14.4" customHeight="1">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="13"/>
@@ -3944,9 +3585,6 @@
       <c r="H84" s="13"/>
     </row>
     <row r="85" ht="14.4" customHeight="1">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="13"/>
@@ -3954,9 +3592,6 @@
       <c r="H85" s="13"/>
     </row>
     <row r="86" ht="14.4" customHeight="1">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="13"/>
@@ -3964,9 +3599,6 @@
       <c r="H86" s="13"/>
     </row>
     <row r="87" ht="14.4" customHeight="1">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="13"/>
@@ -3974,9 +3606,6 @@
       <c r="H87" s="13"/>
     </row>
     <row r="88" ht="14.4" customHeight="1">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="13"/>
@@ -3984,9 +3613,6 @@
       <c r="H88" s="13"/>
     </row>
     <row r="89" ht="14.4" customHeight="1">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="13"/>
@@ -3994,9 +3620,6 @@
       <c r="H89" s="13"/>
     </row>
     <row r="90" ht="14.4" customHeight="1">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="13"/>
@@ -4004,9 +3627,6 @@
       <c r="H90" s="13"/>
     </row>
     <row r="91" ht="14.4" customHeight="1">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="13"/>
@@ -4014,9 +3634,6 @@
       <c r="H91" s="13"/>
     </row>
     <row r="92" ht="14.4" customHeight="1">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="13"/>
@@ -4024,9 +3641,6 @@
       <c r="H92" s="13"/>
     </row>
     <row r="93" ht="14.4" customHeight="1">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="13"/>
@@ -4034,9 +3648,6 @@
       <c r="H93" s="13"/>
     </row>
     <row r="94" ht="14.4" customHeight="1">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="13"/>
@@ -4044,9 +3655,6 @@
       <c r="H94" s="13"/>
     </row>
     <row r="95" ht="14.4" customHeight="1">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="13"/>
@@ -4054,9 +3662,6 @@
       <c r="H95" s="13"/>
     </row>
     <row r="96" ht="14.4" customHeight="1">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="13"/>
@@ -4064,9 +3669,6 @@
       <c r="H96" s="13"/>
     </row>
     <row r="97" ht="14.4" customHeight="1">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="C97"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="13"/>
@@ -4074,538 +3676,252 @@
       <c r="H97" s="13"/>
     </row>
     <row r="98" ht="14.4" customHeight="1">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
     </row>
     <row r="99" ht="14.4" customHeight="1">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
     </row>
     <row r="100" ht="14.4" customHeight="1">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
     </row>
     <row r="101" ht="14.4" customHeight="1">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
     </row>
     <row r="102" ht="14.4" customHeight="1">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
-      <c r="F102" s="13"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="13"/>
     </row>
     <row r="103" ht="14.4" customHeight="1">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="13"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
     </row>
     <row r="104" ht="14.4" customHeight="1">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
-      <c r="F104" s="13"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
     </row>
     <row r="105" ht="14.4" customHeight="1">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
-      <c r="F105" s="13"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
     </row>
     <row r="106" ht="14.4" customHeight="1">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
-      <c r="F106" s="13"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13"/>
     </row>
     <row r="107" ht="14.4" customHeight="1">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
     </row>
     <row r="108" ht="14.4" customHeight="1">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
     </row>
     <row r="109" ht="14.4" customHeight="1">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="C109"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
     </row>
     <row r="110" ht="14.4" customHeight="1">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="C110"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
     </row>
     <row r="111" ht="14.4" customHeight="1">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="C111"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
     </row>
     <row r="112" ht="14.4" customHeight="1">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="C112"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
     </row>
     <row r="113" ht="14.4" customHeight="1">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
     </row>
     <row r="114" ht="14.4" customHeight="1">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
     </row>
     <row r="115" ht="14.4" customHeight="1">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
     </row>
     <row r="116" ht="14.4" customHeight="1">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
     </row>
     <row r="117" ht="14.4" customHeight="1">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
     </row>
     <row r="118" ht="14.4" customHeight="1">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
     </row>
     <row r="119" ht="14.4" customHeight="1">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
     </row>
     <row r="120" ht="14.4" customHeight="1">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
     </row>
     <row r="121" ht="14.4" customHeight="1">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="C121"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
     </row>
     <row r="122" ht="14.4" customHeight="1">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="C122"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
     </row>
     <row r="123" ht="14.4" customHeight="1">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
     </row>
     <row r="124" ht="14.4" customHeight="1">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
     </row>
     <row r="125" ht="14.4" customHeight="1">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="C125"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
     </row>
     <row r="126" ht="14.4" customHeight="1">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="C126"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
     </row>
     <row r="127" ht="14.4" customHeight="1">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="C127"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
     </row>
     <row r="128" ht="14.4" customHeight="1">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="C128"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
     </row>
     <row r="129" ht="14.4" customHeight="1">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="C129"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
     </row>
     <row r="130" ht="14.4" customHeight="1">
-      <c r="A130"/>
-      <c r="B130"/>
-      <c r="C130"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
     </row>
     <row r="131" ht="14.4" customHeight="1">
-      <c r="A131"/>
-      <c r="B131"/>
-      <c r="C131"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
     </row>
     <row r="132" ht="14.4" customHeight="1">
-      <c r="A132"/>
-      <c r="B132"/>
-      <c r="C132"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
     </row>
     <row r="133" ht="14.4" customHeight="1">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="C133"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
     </row>
     <row r="134" ht="14.4" customHeight="1">
-      <c r="A134"/>
-      <c r="B134"/>
-      <c r="C134"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
     </row>
     <row r="135" ht="14.4" customHeight="1">
-      <c r="A135"/>
-      <c r="B135"/>
-      <c r="C135"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
     </row>
     <row r="136" ht="14.4" customHeight="1">
-      <c r="A136"/>
-      <c r="B136"/>
-      <c r="C136"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
     </row>
     <row r="137" ht="14.4" customHeight="1">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="C137"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
     </row>
     <row r="138" ht="14.4" customHeight="1">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="C138"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
     </row>
     <row r="139" ht="14.4" customHeight="1">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="C139"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
     </row>
     <row r="140" ht="14.4" customHeight="1">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="C140"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
     </row>
     <row r="141" ht="14.4" customHeight="1">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="C141"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
     </row>
     <row r="142" ht="14.4" customHeight="1">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="C142"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
     </row>
     <row r="143" ht="14.4" customHeight="1">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="C143"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
     </row>
     <row r="144" ht="14.4" customHeight="1">
-      <c r="A144"/>
-      <c r="B144"/>
-      <c r="C144"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
     </row>
     <row r="145" ht="14.4" customHeight="1">
-      <c r="A145"/>
-      <c r="B145"/>
-      <c r="C145"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
     </row>
     <row r="146" ht="14.4" customHeight="1">
-      <c r="A146"/>
-      <c r="B146"/>
-      <c r="C146"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
     </row>
     <row r="147" ht="14.4" customHeight="1">
-      <c r="A147"/>
-      <c r="B147"/>
-      <c r="C147"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
     </row>
     <row r="148" ht="14.4" customHeight="1">
-      <c r="A148"/>
-      <c r="B148"/>
-      <c r="C148"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
     </row>
     <row r="149" ht="14.4" customHeight="1">
-      <c r="A149"/>
-      <c r="B149"/>
-      <c r="C149"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
     </row>
     <row r="150" ht="14.4" customHeight="1">
-      <c r="A150"/>
-      <c r="B150"/>
-      <c r="C150"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
     </row>
     <row r="151" ht="14.4" customHeight="1">
-      <c r="A151"/>
-      <c r="B151"/>
-      <c r="C151"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
     </row>
     <row r="152" ht="14.4" customHeight="1">
-      <c r="A152"/>
-      <c r="B152"/>
-      <c r="C152"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
     </row>
     <row r="153" ht="14.4" customHeight="1">
-      <c r="A153"/>
-      <c r="B153"/>
-      <c r="C153"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
     </row>
     <row r="154" ht="14.4" customHeight="1">
-      <c r="A154"/>
-      <c r="B154"/>
-      <c r="C154"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
     </row>
     <row r="155" ht="14.4" customHeight="1">
-      <c r="A155"/>
-      <c r="B155"/>
-      <c r="C155"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
     </row>
     <row r="156" ht="14.4" customHeight="1">
-      <c r="A156"/>
-      <c r="B156"/>
-      <c r="C156"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
     </row>
     <row r="157" ht="14.4" customHeight="1">
-      <c r="A157"/>
-      <c r="B157"/>
-      <c r="C157"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
     </row>
     <row r="158" ht="14.4" customHeight="1">
-      <c r="A158"/>
-      <c r="B158"/>
-      <c r="C158"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
     </row>
     <row r="159" ht="14.4" customHeight="1">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="C159"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
-    </row>
-    <row r="160" ht="14.4" customHeight="1">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-    </row>
-    <row r="161" ht="14.4" customHeight="1">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="C161"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-    </row>
-    <row r="162" ht="14.4" customHeight="1">
-      <c r="A162"/>
-      <c r="B162"/>
-      <c r="C162"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="2"/>
-    </row>
-    <row r="163" ht="14.4" customHeight="1">
-      <c r="A163"/>
-      <c r="B163"/>
-      <c r="C163"/>
-      <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
-    </row>
-    <row r="164" ht="14.4" customHeight="1">
-      <c r="A164"/>
-      <c r="B164"/>
-      <c r="C164"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
-    </row>
-    <row r="165" ht="14.4" customHeight="1">
-      <c r="A165"/>
-      <c r="B165"/>
-      <c r="C165"/>
-      <c r="D165" s="2"/>
-      <c r="E165" s="2"/>
-    </row>
-    <row r="166" ht="14.4" customHeight="1">
-      <c r="A166"/>
-      <c r="B166"/>
-      <c r="C166"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
-    </row>
-    <row r="167" ht="14.4" customHeight="1">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="C167"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
-    </row>
-    <row r="168" ht="14.4" customHeight="1">
-      <c r="A168"/>
-      <c r="B168"/>
-      <c r="C168"/>
-      <c r="D168" s="2"/>
-      <c r="E168" s="2"/>
-    </row>
-    <row r="169" ht="14.4" customHeight="1">
-      <c r="A169"/>
-      <c r="B169"/>
-      <c r="C169"/>
-      <c r="D169" s="2"/>
-      <c r="E169" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -4666,45 +3982,45 @@
         <v>2</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="O1" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" ht="15.6">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1">
         <v>-2.7833329999999998</v>
@@ -4745,7 +4061,7 @@
     </row>
     <row r="3" ht="15.6">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1">
         <v>-6.4666670000000002</v>
@@ -4786,7 +4102,7 @@
     </row>
     <row r="4" ht="15.6">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1">
         <v>-4.7000000000000002</v>
@@ -4827,7 +4143,7 @@
     </row>
     <row r="5" ht="15.6">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1">
         <v>-5.3499999999999996</v>
@@ -4868,7 +4184,7 @@
     </row>
     <row r="6" ht="15.6">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1">
         <v>-5.9500000000000002</v>
@@ -4909,7 +4225,7 @@
     </row>
     <row r="7" ht="15.6">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1">
         <v>-3.2999999999999998</v>
@@ -4950,7 +4266,7 @@
     </row>
     <row r="8" ht="15.6">
       <c r="A8" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1">
         <v>-3.9333330000000002</v>
@@ -4991,7 +4307,7 @@
     </row>
     <row r="9" ht="15.6">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1">
         <v>-6.0833329999999997</v>
@@ -5032,7 +4348,7 @@
     </row>
     <row r="10" ht="15.6">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1">
         <v>-6.6500000000000004</v>
@@ -5073,7 +4389,7 @@
     </row>
     <row r="11" ht="15.6">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B11" s="1">
         <v>-7.3666669999999996</v>
@@ -5114,7 +4430,7 @@
     </row>
     <row r="12" ht="14.4">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1">
         <v>-7.5666669999999998</v>
@@ -5155,7 +4471,7 @@
     </row>
     <row r="13" ht="14.4">
       <c r="A13" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1">
         <v>-7.516667</v>
@@ -5196,7 +4512,7 @@
     </row>
     <row r="14" ht="14.4">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1">
         <v>-5.0666669999999998</v>
@@ -5237,7 +4553,7 @@
     </row>
     <row r="15" ht="14.4">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1">
         <v>-5.6166669999999996</v>
@@ -5278,7 +4594,7 @@
     </row>
     <row r="16" ht="14.4">
       <c r="A16" s="34" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1">
         <v>-4.6200000000000001</v>
@@ -5301,7 +4617,7 @@
     </row>
     <row r="17" ht="14.4">
       <c r="A17" s="34" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1">
         <v>-6.0199999999999996</v>
@@ -5324,7 +4640,7 @@
     </row>
     <row r="18" ht="14.4">
       <c r="A18" s="34" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B18" s="1">
         <v>-4.4800000000000004</v>
@@ -5347,7 +4663,7 @@
     </row>
     <row r="19" ht="14.4">
       <c r="A19" s="34" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1">
         <v>-6.5199999999999996</v>
@@ -5370,7 +4686,7 @@
     </row>
     <row r="20" ht="14.4">
       <c r="A20" s="34" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1">
         <v>-3.4700000000000002</v>
@@ -5393,7 +4709,7 @@
     </row>
     <row r="21" ht="14.4">
       <c r="A21" s="34" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1">
         <v>-7.5499999999999998</v>
@@ -5416,7 +4732,7 @@
     </row>
     <row r="22" ht="14.4">
       <c r="A22" s="34" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1">
         <v>-8.0600000000000005</v>
@@ -5439,7 +4755,7 @@
     </row>
     <row r="23" ht="14.4">
       <c r="A23" s="34" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1">
         <v>-3.3399999999999999</v>
@@ -5462,7 +4778,7 @@
     </row>
     <row r="24" ht="14.4">
       <c r="A24" s="34" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1">
         <v>-3.4666670000000002</v>
@@ -5485,7 +4801,7 @@
     </row>
     <row r="25" ht="14.4">
       <c r="A25" s="34" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1">
         <v>-3.1666669999999999</v>
@@ -5508,7 +4824,7 @@
     </row>
     <row r="26" ht="14.4">
       <c r="A26" s="34" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B26" s="1">
         <v>-5.2999999999999998</v>
@@ -5531,7 +4847,7 @@
     </row>
     <row r="27" ht="14.4">
       <c r="A27" s="34" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B27" s="1">
         <v>-5.2833329999999998</v>
@@ -5554,7 +4870,7 @@
     </row>
     <row r="28" ht="14.4">
       <c r="A28" s="34" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1">
         <v>-5.4000000000000004</v>
@@ -5577,7 +4893,7 @@
     </row>
     <row r="29" ht="14.4">
       <c r="A29" s="34" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B29" s="64">
         <v>-5.1500000000000004</v>
@@ -5600,7 +4916,7 @@
     </row>
     <row r="30" ht="14.4">
       <c r="A30" s="34" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1">
         <v>-5.4166670000000003</v>
@@ -5623,7 +4939,7 @@
     </row>
     <row r="31" ht="14.4">
       <c r="A31" s="34" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1">
         <v>-7.8166669999999998</v>
@@ -5646,7 +4962,7 @@
     </row>
     <row r="32" ht="14.4">
       <c r="A32" s="34" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B32" s="1">
         <v>-7.3833330000000004</v>
@@ -5669,7 +4985,7 @@
     </row>
     <row r="33" ht="14.4">
       <c r="A33" s="65" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B33" s="1">
         <v>-4.8333329999999997</v>
@@ -5692,7 +5008,7 @@
     </row>
     <row r="34" ht="14.4">
       <c r="A34" s="34" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B34" s="66">
         <v>-5.75</v>
@@ -5715,7 +5031,7 @@
     </row>
     <row r="35" ht="14.4">
       <c r="A35" s="34" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B35" s="1">
         <v>-6.5999999999999996</v>
@@ -5738,7 +5054,7 @@
     </row>
     <row r="36" ht="14.4">
       <c r="A36" s="34" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B36" s="1">
         <v>-6.5999999999999996</v>
@@ -5761,7 +5077,7 @@
     </row>
     <row r="37" ht="14.4">
       <c r="A37" s="34" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1">
         <v>-6.0666669999999998</v>
@@ -5784,7 +5100,7 @@
     </row>
     <row r="38" ht="14.4">
       <c r="A38" s="34" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B38" s="1">
         <v>-4.516667</v>
@@ -5807,7 +5123,7 @@
     </row>
     <row r="39" ht="14.4">
       <c r="A39" s="34" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1">
         <v>-4.3666669999999996</v>
@@ -5830,7 +5146,7 @@
     </row>
     <row r="40" ht="14.4">
       <c r="A40" s="34" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B40" s="1">
         <v>-4.2000000000000002</v>
@@ -5853,7 +5169,7 @@
     </row>
     <row r="41" ht="14.4">
       <c r="A41" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B41" s="1">
         <v>-3.2000000000000002</v>
@@ -5876,7 +5192,7 @@
     </row>
     <row r="42" ht="14.4">
       <c r="A42" s="34" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B42" s="1">
         <v>-3.6000000000000001</v>
@@ -5899,7 +5215,7 @@
     </row>
     <row r="43" ht="14.4">
       <c r="A43" s="34" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1">
         <v>-5.9166670000000003</v>
@@ -5922,7 +5238,7 @@
     </row>
     <row r="44" ht="14.4">
       <c r="A44" s="34" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1">
         <v>-5.0499999999999998</v>
@@ -5945,7 +5261,7 @@
     </row>
     <row r="45" ht="14.4">
       <c r="A45" s="34" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B45" s="1">
         <v>-4.3666669999999996</v>
@@ -5968,7 +5284,7 @@
     </row>
     <row r="46" ht="14.4">
       <c r="A46" s="34" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1">
         <v>-3.9500000000000002</v>
@@ -5991,7 +5307,7 @@
     </row>
     <row r="47" ht="14.4">
       <c r="A47" s="34" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1">
         <v>-5.016667</v>
@@ -6014,7 +5330,7 @@
     </row>
     <row r="48" ht="14.4">
       <c r="A48" s="34" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B48" s="1">
         <v>-5.5833329999999997</v>
@@ -6037,7 +5353,7 @@
     </row>
     <row r="49" ht="14.4">
       <c r="A49" s="34" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B49" s="64">
         <v>-3.3833329999999999</v>
@@ -6060,7 +5376,7 @@
     </row>
     <row r="50" ht="14.4">
       <c r="A50" s="67" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B50" s="67">
         <v>-6.25</v>
@@ -6071,7 +5387,7 @@
     </row>
     <row r="51" ht="14.4">
       <c r="A51" s="67" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B51" s="67">
         <v>-7.233333</v>
@@ -6082,7 +5398,7 @@
     </row>
     <row r="52" ht="14.4">
       <c r="A52" s="67" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B52" s="67">
         <v>-3.3166669999999998</v>
@@ -6093,7 +5409,7 @@
     </row>
     <row r="53" ht="14.4">
       <c r="A53" s="67" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B53" s="67">
         <v>-5.9000000000000004</v>
@@ -6104,7 +5420,7 @@
     </row>
     <row r="54" ht="14.4">
       <c r="A54" s="67" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B54" s="67">
         <v>-5.1500000000000004</v>
@@ -6115,7 +5431,7 @@
     </row>
     <row r="55" ht="14.4">
       <c r="A55" s="67" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B55" s="67">
         <v>-4.99305555555555</v>
@@ -6126,7 +5442,7 @@
     </row>
     <row r="56" ht="14.4">
       <c r="A56" s="67" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B56" s="67">
         <v>-7.4000000000000004</v>
@@ -6137,7 +5453,7 @@
     </row>
     <row r="57" ht="14.4">
       <c r="A57" s="67" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B57" s="67">
         <v>-6.4666670000000002</v>
@@ -6159,7 +5475,7 @@
     </row>
     <row r="59" ht="14.4">
       <c r="A59" s="67" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B59" s="67">
         <v>-5.2254300000000002</v>
@@ -6170,7 +5486,7 @@
     </row>
     <row r="60" ht="14.4">
       <c r="A60" s="67" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B60" s="67">
         <v>-4.0113690000000002</v>
@@ -6192,7 +5508,7 @@
     </row>
     <row r="62" ht="14.4">
       <c r="A62" s="67" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B62" s="67">
         <v>-6.4097200000000001</v>
@@ -6203,7 +5519,7 @@
     </row>
     <row r="63" ht="14.4">
       <c r="A63" s="67" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B63" s="67">
         <v>-3.3748</v>
@@ -6256,45 +5572,45 @@
         <v>2</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="O1" s="33" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" ht="15">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1">
         <v>-2.7833329999999998</v>
@@ -6335,7 +5651,7 @@
     </row>
     <row r="3" ht="15">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1">
         <v>-6.4666670000000002</v>
@@ -6376,7 +5692,7 @@
     </row>
     <row r="4" ht="15">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1">
         <v>-4.7000000000000002</v>
@@ -6417,7 +5733,7 @@
     </row>
     <row r="5" ht="15">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1">
         <v>-5.3499999999999996</v>
@@ -6458,7 +5774,7 @@
     </row>
     <row r="6" ht="15">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1">
         <v>-5.9500000000000002</v>
@@ -6499,7 +5815,7 @@
     </row>
     <row r="7" ht="15">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1">
         <v>-3.2999999999999998</v>
@@ -6540,7 +5856,7 @@
     </row>
     <row r="8" ht="15">
       <c r="A8" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1">
         <v>-3.9333330000000002</v>
@@ -6581,7 +5897,7 @@
     </row>
     <row r="9" ht="15">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1">
         <v>-6.0833329999999997</v>
@@ -6622,7 +5938,7 @@
     </row>
     <row r="10" ht="15">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1">
         <v>-6.6500000000000004</v>
@@ -6663,7 +5979,7 @@
     </row>
     <row r="11" ht="15">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B11" s="1">
         <v>-7.3666669999999996</v>
@@ -6704,7 +6020,7 @@
     </row>
     <row r="12" ht="14.4">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1">
         <v>-7.5666669999999998</v>
@@ -6745,7 +6061,7 @@
     </row>
     <row r="13" ht="14.4">
       <c r="A13" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1">
         <v>-7.516667</v>
@@ -6786,7 +6102,7 @@
     </row>
     <row r="14" ht="14.4">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1">
         <v>-5.0666669999999998</v>
@@ -6827,7 +6143,7 @@
     </row>
     <row r="15" ht="14.4">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1">
         <v>-5.6166669999999996</v>
@@ -6868,7 +6184,7 @@
     </row>
     <row r="16" ht="14.4">
       <c r="A16" s="34" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1">
         <v>-4.6200000000000001</v>
@@ -6891,7 +6207,7 @@
     </row>
     <row r="17" ht="14.4">
       <c r="A17" s="34" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1">
         <v>-6.0199999999999996</v>
@@ -6914,7 +6230,7 @@
     </row>
     <row r="18" ht="14.4">
       <c r="A18" s="34" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B18" s="1">
         <v>-4.4800000000000004</v>
@@ -6937,7 +6253,7 @@
     </row>
     <row r="19" ht="14.4">
       <c r="A19" s="34" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1">
         <v>-6.5199999999999996</v>
@@ -6960,7 +6276,7 @@
     </row>
     <row r="20" ht="14.4">
       <c r="A20" s="34" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1">
         <v>-3.4700000000000002</v>
@@ -6983,7 +6299,7 @@
     </row>
     <row r="21" ht="14.4">
       <c r="A21" s="34" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1">
         <v>-7.5499999999999998</v>
@@ -7006,7 +6322,7 @@
     </row>
     <row r="22" ht="14.4">
       <c r="A22" s="34" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1">
         <v>-8.0600000000000005</v>
@@ -7029,7 +6345,7 @@
     </row>
     <row r="23" ht="14.4">
       <c r="A23" s="34" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1">
         <v>-3.3399999999999999</v>
@@ -7052,7 +6368,7 @@
     </row>
     <row r="24" ht="14.4">
       <c r="A24" s="34" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1">
         <v>-3.4666670000000002</v>
@@ -7075,7 +6391,7 @@
     </row>
     <row r="25" ht="14.4">
       <c r="A25" s="34" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1">
         <v>-3.1666669999999999</v>
@@ -7098,7 +6414,7 @@
     </row>
     <row r="26" ht="14.4">
       <c r="A26" s="34" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B26" s="1">
         <v>-5.2999999999999998</v>
@@ -7121,7 +6437,7 @@
     </row>
     <row r="27" ht="14.4">
       <c r="A27" s="34" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B27" s="1">
         <v>-5.2833329999999998</v>
@@ -7144,7 +6460,7 @@
     </row>
     <row r="28" ht="14.4">
       <c r="A28" s="34" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1">
         <v>-5.4000000000000004</v>
@@ -7167,7 +6483,7 @@
     </row>
     <row r="29" ht="14.4">
       <c r="A29" s="34" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B29" s="64">
         <v>-5.1500000000000004</v>
@@ -7190,7 +6506,7 @@
     </row>
     <row r="30" ht="14.4">
       <c r="A30" s="34" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1">
         <v>-5.4166670000000003</v>
@@ -7213,7 +6529,7 @@
     </row>
     <row r="31" ht="14.4">
       <c r="A31" s="34" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1">
         <v>-7.8166669999999998</v>
@@ -7236,7 +6552,7 @@
     </row>
     <row r="32" ht="14.4">
       <c r="A32" s="34" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B32" s="1">
         <v>-7.3833330000000004</v>
@@ -7259,7 +6575,7 @@
     </row>
     <row r="33" ht="14.4">
       <c r="A33" s="65" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B33" s="1">
         <v>-4.8333329999999997</v>
@@ -7282,7 +6598,7 @@
     </row>
     <row r="34" ht="14.4">
       <c r="A34" s="34" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B34" s="66">
         <v>-5.75</v>
@@ -7305,7 +6621,7 @@
     </row>
     <row r="35" ht="14.4">
       <c r="A35" s="34" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B35" s="1">
         <v>-6.5999999999999996</v>
@@ -7328,7 +6644,7 @@
     </row>
     <row r="36" ht="14.4">
       <c r="A36" s="34" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B36" s="1">
         <v>-6.5999999999999996</v>
@@ -7351,7 +6667,7 @@
     </row>
     <row r="37" ht="14.4">
       <c r="A37" s="34" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1">
         <v>-6.0666669999999998</v>
@@ -7374,7 +6690,7 @@
     </row>
     <row r="38" ht="14.4">
       <c r="A38" s="34" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B38" s="1">
         <v>-4.516667</v>
@@ -7397,7 +6713,7 @@
     </row>
     <row r="39" ht="14.4">
       <c r="A39" s="34" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1">
         <v>-4.3666669999999996</v>
@@ -7420,7 +6736,7 @@
     </row>
     <row r="40" ht="14.4">
       <c r="A40" s="34" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B40" s="1">
         <v>-4.2000000000000002</v>
@@ -7443,7 +6759,7 @@
     </row>
     <row r="41" ht="14.4">
       <c r="A41" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B41" s="1">
         <v>-3.2000000000000002</v>
@@ -7466,7 +6782,7 @@
     </row>
     <row r="42" ht="14.4">
       <c r="A42" s="34" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B42" s="1">
         <v>-3.6000000000000001</v>
@@ -7489,7 +6805,7 @@
     </row>
     <row r="43" ht="14.4">
       <c r="A43" s="34" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1">
         <v>-5.9166670000000003</v>
@@ -7512,7 +6828,7 @@
     </row>
     <row r="44" ht="14.4">
       <c r="A44" s="34" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B44" s="1">
         <v>-5.0499999999999998</v>
@@ -7535,7 +6851,7 @@
     </row>
     <row r="45" ht="14.4">
       <c r="A45" s="34" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B45" s="1">
         <v>-4.3666669999999996</v>
@@ -7558,7 +6874,7 @@
     </row>
     <row r="46" ht="14.4">
       <c r="A46" s="34" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1">
         <v>-3.9500000000000002</v>
@@ -7581,7 +6897,7 @@
     </row>
     <row r="47" ht="14.4">
       <c r="A47" s="34" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1">
         <v>-5.016667</v>
@@ -7604,7 +6920,7 @@
     </row>
     <row r="48" ht="14.4">
       <c r="A48" s="34" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B48" s="1">
         <v>-5.5833329999999997</v>
@@ -7627,7 +6943,7 @@
     </row>
     <row r="49" ht="14.4">
       <c r="A49" s="34" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B49" s="64">
         <v>-3.3833329999999999</v>
@@ -7650,7 +6966,7 @@
     </row>
     <row r="50" ht="14.4">
       <c r="A50" s="67" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B50" s="67">
         <v>-6.25</v>
@@ -7661,7 +6977,7 @@
     </row>
     <row r="51" ht="14.4">
       <c r="A51" s="67" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B51" s="67">
         <v>-7.233333</v>
@@ -7672,7 +6988,7 @@
     </row>
     <row r="52" ht="14.4">
       <c r="A52" s="67" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B52" s="67">
         <v>-3.3166669999999998</v>
@@ -7683,7 +6999,7 @@
     </row>
     <row r="53" ht="14.4">
       <c r="A53" s="67" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B53" s="67">
         <v>-5.9000000000000004</v>
@@ -7694,7 +7010,7 @@
     </row>
     <row r="54" ht="14.4">
       <c r="A54" s="67" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B54" s="67">
         <v>-5.1500000000000004</v>
@@ -7705,7 +7021,7 @@
     </row>
     <row r="55" ht="14.4">
       <c r="A55" s="67" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B55" s="67">
         <v>-4.99305555555555</v>
@@ -7716,7 +7032,7 @@
     </row>
     <row r="56" ht="14.4">
       <c r="A56" s="67" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B56" s="67">
         <v>-7.4000000000000004</v>
@@ -7727,7 +7043,7 @@
     </row>
     <row r="57" ht="14.4">
       <c r="A57" s="67" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B57" s="67">
         <v>-6.4666670000000002</v>
@@ -7749,7 +7065,7 @@
     </row>
     <row r="59" ht="14.4">
       <c r="A59" s="67" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B59" s="67">
         <v>-5.2254300000000002</v>
@@ -7760,7 +7076,7 @@
     </row>
     <row r="60" ht="14.4">
       <c r="A60" s="67" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B60" s="67">
         <v>-4.0113690000000002</v>
@@ -7782,7 +7098,7 @@
     </row>
     <row r="62" ht="14.4">
       <c r="A62" s="67" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B62" s="67">
         <v>-6.4097200000000001</v>
@@ -7793,7 +7109,7 @@
     </row>
     <row r="63" ht="14.4">
       <c r="A63" s="67" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B63" s="67">
         <v>-3.3748</v>

</xml_diff>